<commit_message>
Update MYPROFILE and edit Information test cases
</commit_message>
<xml_diff>
--- a/Car_TestCases/Car_Myprofile_and_editinformation.xlsx
+++ b/Car_TestCases/Car_Myprofile_and_editinformation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>Test case ID</t>
   </si>
@@ -85,30 +85,6 @@
   </si>
   <si>
     <t>Car_MyProfile_03</t>
-  </si>
-  <si>
-    <t>Car_MyProfile_04</t>
-  </si>
-  <si>
-    <t>Car_MyProfile_05</t>
-  </si>
-  <si>
-    <t>Car_MyProfile_06</t>
-  </si>
-  <si>
-    <t>Car_MyProfile_07</t>
-  </si>
-  <si>
-    <t>Car_MyProfile_08</t>
-  </si>
-  <si>
-    <t>Car_MyProfile_09</t>
-  </si>
-  <si>
-    <t>Car_MyProfile_10</t>
-  </si>
-  <si>
-    <t>Car_MyProfile_11</t>
   </si>
   <si>
     <t>Validate "MY PROFILE" functionality</t>
@@ -175,12 +151,21 @@
   <si>
     <t>Failed</t>
   </si>
+  <si>
+    <t>Car_EditInformation_01</t>
+  </si>
+  <si>
+    <t>Car_EditInformation_02</t>
+  </si>
+  <si>
+    <t>Edit Information</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,8 +184,16 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,6 +203,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -226,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -239,6 +238,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -631,15 +639,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="151.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" style="3" customWidth="1"/>
     <col min="2" max="2" width="20.140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="34" style="3" customWidth="1"/>
@@ -718,7 +726,7 @@
         <v>19</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -729,25 +737,25 @@
         <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -755,126 +763,121 @@
         <v>22</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>19</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>44</v>
-      </c>
+    <row r="5" spans="1:13" s="6" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
     </row>
     <row r="6" spans="1:13" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>25</v>
+        <v>39</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="K7" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="J8" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>30</v>
+      <c r="J9" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:M5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update My profile and edit information test cases
</commit_message>
<xml_diff>
--- a/Car_TestCases/Car_Myprofile_and_editinformation.xlsx
+++ b/Car_TestCases/Car_Myprofile_and_editinformation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t>Test case ID</t>
   </si>
@@ -95,16 +95,7 @@
 3)Click on My Profile button</t>
   </si>
   <si>
-    <t>User should be redirct to My Profile  page witch contain his information (Name, Email, Address, Phone)</t>
-  </si>
-  <si>
-    <t>Function</t>
-  </si>
-  <si>
     <t>Car_SRS_25</t>
-  </si>
-  <si>
-    <t>Valide UI of MY PROFILE page</t>
   </si>
   <si>
     <t>Form displayed with 4 text fields   
@@ -159,6 +150,15 @@
   </si>
   <si>
     <t>Edit Information</t>
+  </si>
+  <si>
+    <t>User should be redirected to My Profile  page which contains his information (Name, Email, Address, Phone)</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>Validate UI of MY PROFILE page</t>
   </si>
 </sst>
 </file>
@@ -240,12 +240,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -270,22 +270,20 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>39418</xdr:colOff>
+      <xdr:colOff>57151</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>2659111</xdr:colOff>
+      <xdr:colOff>2686051</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1866900</xdr:rowOff>
+      <xdr:rowOff>1835150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
@@ -301,46 +299,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14003068" y="352425"/>
-          <a:ext cx="2619693" cy="1800225"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>80096</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>2695575</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>1876425</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14058900" y="4252046"/>
-          <a:ext cx="2600325" cy="1796329"/>
+          <a:off x="14363701" y="381000"/>
+          <a:ext cx="2628900" cy="1778000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -639,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="H4" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="151.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -726,7 +686,7 @@
         <v>19</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -737,7 +697,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>23</v>
@@ -749,13 +709,13 @@
         <v>24</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -763,13 +723,13 @@
         <v>22</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>16</v>
@@ -778,98 +738,88 @@
         <v>24</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>19</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="6" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
+    <row r="5" spans="1:13" s="5" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
     </row>
     <row r="6" spans="1:13" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J8" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J9" s="3" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>